<commit_message>
Updated Triangle to change it back to a 100 size (as a test) since it's all the same pattern right now - not as impressive.  But - that will change in a sec.
</commit_message>
<xml_diff>
--- a/SSoT/twolaat.xlsx
+++ b/SSoT/twolaat.xlsx
@@ -19,7 +19,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="116">
   <si>
+    <t>WayNumber</t>
+  </si>
+  <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Advantages</t>
+  </si>
+  <si>
+    <t>Disadvantages</t>
+  </si>
+  <si>
+    <t>HexValue</t>
   </si>
   <si>
     <t>Type</t>
@@ -28,16 +43,13 @@
     <t>InitialValue</t>
   </si>
   <si>
-    <t>WayNumber</t>
-  </si>
-  <si>
-    <t>HexValue</t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
     <t>Black</t>
+  </si>
+  <si>
+    <t>W01</t>
   </si>
   <si>
     <t>#000000</t>
@@ -46,19 +58,10 @@
     <t>0x0</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
-    <t>Advantages</t>
-  </si>
-  <si>
     <t>#FF0000</t>
-  </si>
-  <si>
-    <t>Disadvantages</t>
   </si>
   <si>
     <t>Blue</t>
@@ -70,22 +73,13 @@
     <t>Green</t>
   </si>
   <si>
-    <t>W01</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
-    <t>Degrees</t>
-  </si>
-  <si>
     <t>OOTurtle</t>
   </si>
   <si>
     <t>I'm</t>
   </si>
   <si>
-    <t>Color</t>
+    <t>#00FF00</t>
   </si>
   <si>
     <t>not</t>
@@ -101,9 +95,6 @@
   </si>
   <si>
     <t>to</t>
-  </si>
-  <si>
-    <t>PenState</t>
   </si>
   <si>
     <t>copy</t>
@@ -127,10 +118,22 @@
     <t>list</t>
   </si>
   <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
     <t>W04</t>
   </si>
   <si>
     <t>Api_FP_Core</t>
+  </si>
+  <si>
+    <t>PenState</t>
   </si>
   <si>
     <t>in</t>
@@ -163,13 +166,13 @@
     <t>DependencyInjection_Interface-1</t>
   </si>
   <si>
+    <t>Down</t>
+  </si>
+  <si>
     <t>then</t>
   </si>
   <si>
     <t>the</t>
-  </si>
-  <si>
-    <t>#00FF00</t>
   </si>
   <si>
     <t>structure</t>
@@ -221,9 +224,6 @@
   </si>
   <si>
     <t>list.</t>
-  </si>
-  <si>
-    <t>Down</t>
   </si>
   <si>
     <t>W09</t>
@@ -412,14 +412,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -446,31 +446,31 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,21 +488,21 @@
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -510,7 +510,7 @@
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -564,20 +564,20 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -602,175 +602,175 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>17</v>
+      <c r="A2" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="7" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="C7" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="D7" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>46</v>
+      <c r="A8" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>64</v>
+      <c r="A11" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -781,7 +781,7 @@
       <c r="E12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -792,7 +792,7 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -803,7 +803,7 @@
       <c r="E14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -814,7 +814,7 @@
       <c r="E15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -825,7 +825,7 @@
       <c r="E16" s="11"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -836,7 +836,7 @@
       <c r="E17" s="11"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -847,7 +847,7 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -6756,14 +6756,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -6791,21 +6791,21 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7">
         <v>0.0</v>
@@ -6813,24 +6813,24 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
+      <c r="C4" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>28</v>
+      <c r="B5" s="10" t="s">
+        <v>38</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>68</v>
+      <c r="C5" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6">
@@ -9834,11 +9834,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9866,58 +9866,58 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>50</v>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -9939,10 +9939,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -9979,43 +9979,43 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -10033,13 +10033,13 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D1" s="3"/>
@@ -10082,7 +10082,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -10100,40 +10100,40 @@
         <v>96</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -10156,13 +10156,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>99</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>100</v>
@@ -10219,40 +10219,40 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="8" t="b">
+      <c r="D4" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -10288,7 +10288,7 @@
         <v>110</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>111</v>
@@ -10325,7 +10325,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="19">
-        <v>150.0</v>
+        <v>100.0</v>
       </c>
       <c r="E2" s="20" t="str">
         <f>vlookup(B2,TurtleCommands!A$2:C7,3,false)</f>
@@ -10401,7 +10401,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="19">
-        <v>150.0</v>
+        <v>100.0</v>
       </c>
       <c r="E4" s="20" t="str">
         <f>vlookup(B4,TurtleCommands!A$2:C9,3,false)</f>
@@ -10477,7 +10477,7 @@
         <v>90</v>
       </c>
       <c r="C6" s="19">
-        <v>150.0</v>
+        <v>100.0</v>
       </c>
       <c r="E6" s="20" t="str">
         <f>vlookup(B6,TurtleCommands!A$2:C11,3,false)</f>
@@ -10592,7 +10592,7 @@
         <v>96</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="20" t="str">
@@ -10865,7 +10865,7 @@
         <v>96</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="20" t="str">
@@ -11138,7 +11138,7 @@
         <v>96</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="20" t="str">
@@ -11247,17 +11247,17 @@
       <c r="AA25" s="24"/>
     </row>
     <row r="26">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C26" s="28">
         <v>100.0</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="8"/>
       <c r="E26" s="20" t="str">
         <f>vlookup(B26,TurtleCommands!A$2:C31,3,false)</f>
         <v>Distance</v>
@@ -11286,17 +11286,17 @@
       <c r="AA26" s="21"/>
     </row>
     <row r="27">
-      <c r="A27" s="8" t="str">
+      <c r="A27" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C27" s="28">
         <v>90.0</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="20" t="str">
         <f>vlookup(B27,TurtleCommands!A$2:C32,3,false)</f>
         <v>Degrees</v>
@@ -11325,17 +11325,17 @@
       <c r="AA27" s="21"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C28" s="28">
         <v>100.0</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="8"/>
       <c r="E28" s="20" t="str">
         <f>vlookup(B28,TurtleCommands!A$2:C33,3,false)</f>
         <v>Distance</v>
@@ -11364,17 +11364,17 @@
       <c r="AA28" s="21"/>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="str">
+      <c r="A29" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C29" s="28">
         <v>90.0</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="8"/>
       <c r="E29" s="20" t="str">
         <f>vlookup(B29,TurtleCommands!A$2:C34,3,false)</f>
         <v>Degrees</v>
@@ -11403,17 +11403,17 @@
       <c r="AA29" s="21"/>
     </row>
     <row r="30">
-      <c r="A30" s="8" t="str">
+      <c r="A30" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="28">
         <v>100.0</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="8"/>
       <c r="E30" s="20" t="str">
         <f>vlookup(B30,TurtleCommands!A$2:C35,3,false)</f>
         <v>Distance</v>
@@ -11442,17 +11442,17 @@
       <c r="AA30" s="21"/>
     </row>
     <row r="31">
-      <c r="A31" s="8" t="str">
+      <c r="A31" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C31" s="28">
         <v>90.0</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="8"/>
       <c r="E31" s="20" t="str">
         <f>vlookup(B31,TurtleCommands!A$2:C36,3,false)</f>
         <v>Degrees</v>
@@ -11481,17 +11481,17 @@
       <c r="AA31" s="21"/>
     </row>
     <row r="32">
-      <c r="A32" s="8" t="str">
+      <c r="A32" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C32" s="28">
         <v>100.0</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="20" t="str">
         <f>vlookup(B32,TurtleCommands!A$2:C37,3,false)</f>
         <v>Distance</v>
@@ -11520,17 +11520,17 @@
       <c r="AA32" s="21"/>
     </row>
     <row r="33">
-      <c r="A33" s="8" t="str">
+      <c r="A33" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="28">
         <v>90.0</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="20" t="str">
         <f>vlookup(B33,TurtleCommands!A$2:C38,3,false)</f>
         <v>Degrees</v>

</xml_diff>

<commit_message>
About to convert C# W02 into a tool.
</commit_message>
<xml_diff>
--- a/SSoT/twolaat.xlsx
+++ b/SSoT/twolaat.xlsx
@@ -22,19 +22,16 @@
     <t>Name</t>
   </si>
   <si>
-    <t>HexValue</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>InitialValue</t>
   </si>
   <si>
     <t>WayNumber</t>
   </si>
   <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>InitialValue</t>
+    <t>HexValue</t>
   </si>
   <si>
     <t>DisplayWayNumber</t>
@@ -46,10 +43,31 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Advantages</t>
+  </si>
+  <si>
+    <t>Disadvantages</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>W01</t>
+  </si>
+  <si>
     <t>#000000</t>
   </si>
   <si>
     <t>Red</t>
+  </si>
+  <si>
+    <t>0x0</t>
   </si>
   <si>
     <t>#FF0000</t>
@@ -64,21 +82,6 @@
     <t>Green</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Advantages</t>
-  </si>
-  <si>
-    <t>Disadvantages</t>
-  </si>
-  <si>
-    <t>W01</t>
-  </si>
-  <si>
-    <t>#00FF00</t>
-  </si>
-  <si>
     <t>Way 01</t>
   </si>
   <si>
@@ -91,11 +94,23 @@
     <t>Simple OO -- a class with mutable state</t>
   </si>
   <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
     <t>In this design, a simple OO class represents the turtle,
 and the client talks to the turtle directly.</t>
   </si>
   <si>
+    <t>Color</t>
+  </si>
+  <si>
     <t>W02</t>
+  </si>
+  <si>
+    <t>PenState</t>
   </si>
   <si>
     <t>Way 02</t>
@@ -108,12 +123,6 @@
   </si>
   <si>
     <t>Simple FP - a module of functions with immutable state</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>0x0</t>
   </si>
   <si>
     <t>In this design, the turtle state is immutable. A module contains functions that return a new turtle state,
@@ -134,6 +143,9 @@
   </si>
   <si>
     <t>API (OO Approach) -- OO API calling stateful core class</t>
+  </si>
+  <si>
+    <t>#00FF00</t>
   </si>
   <si>
     <t>In this design, an API layer communicates with a turtle class
@@ -164,18 +176,6 @@
   </si>
   <si>
     <t>W05</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
-    <t>Degrees</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>PenState</t>
   </si>
   <si>
     <t>Down</t>
@@ -373,6 +373,12 @@
     <t>Abstract Data Turtle - a private type with an associated module of functions</t>
   </si>
   <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>The pen is up (not drawing)</t>
+  </si>
+  <si>
     <t>In this design, the details of the turtle structure is hidden from the client,
 so the it could be changed without breaking any code.
 See https://www.reddit.com/r/fsharp/comments/36s0zr/structuring_f_programs_with_abstract_data_types/?
@@ -380,6 +386,15 @@
   </si>
   <si>
     <t>W15</t>
+  </si>
+  <si>
+    <t>The pne is down (drawing)</t>
+  </si>
+  <si>
+    <t>Moving</t>
+  </si>
+  <si>
+    <t>The pen is in motion</t>
   </si>
   <si>
     <t>15-CapabilityBasedTurtle.fsx</t>
@@ -394,21 +409,6 @@
     <t>In this design, the turtle exposes a list of functions (capabilities) after each action.
 These are the ONLY actions available to the client
 More on capability-based security at http://fsharpforfunandprofit.com/posts/capability-based-security/</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>The pen is up (not drawing)</t>
-  </si>
-  <si>
-    <t>The pne is down (drawing)</t>
-  </si>
-  <si>
-    <t>Moving</t>
-  </si>
-  <si>
-    <t>The pen is in motion</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -549,14 +549,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
@@ -585,35 +585,35 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -634,27 +634,27 @@
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -662,7 +662,7 @@
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -718,493 +718,493 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
+      <c r="A1" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>15</v>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>16</v>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>17</v>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>18</v>
+      <c r="A2" s="6" t="s">
+        <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="F3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="F4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="4" t="str">
+      <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="5" t="str">
         <f t="shared" ref="B6:B19" si="1">CONCATENATE("Way ",right(A6,2))</f>
         <v>Way 05</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="4" t="str">
+      <c r="B7" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 06</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="4" t="str">
+      <c r="B8" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 06</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="4" t="str">
+      <c r="B9" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 07</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="4" t="str">
+      <c r="B10" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 07</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="4" t="str">
+      <c r="B11" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 08</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="13"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="4" t="str">
+      <c r="B12" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 09</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>80</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="4" t="str">
+      <c r="B13" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="4" t="str">
+      <c r="B14" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 11</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>90</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="4" t="str">
+      <c r="B15" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 12</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>95</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="4" t="str">
+      <c r="B16" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 13</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>100</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="4" t="str">
+      <c r="B17" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 13</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>100</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="4" t="str">
+      <c r="B18" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 14</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>107</v>
+      <c r="F18" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
-        <v>108</v>
+      <c r="A19" s="6" t="s">
+        <v>110</v>
       </c>
-      <c r="B19" s="4" t="str">
+      <c r="B19" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 15</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>109</v>
+      <c r="C19" s="5" t="s">
+        <v>114</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>110</v>
+      <c r="D19" s="5" t="s">
+        <v>115</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>111</v>
+      <c r="E19" s="8" t="s">
+        <v>116</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>112</v>
+      <c r="F19" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
     <row r="20">
       <c r="A20" s="13"/>
-      <c r="E20" s="9"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="16"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21">
       <c r="A21" s="13"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="16"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
     <row r="22">
       <c r="A22" s="13"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="16"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
     <row r="23">
       <c r="A23" s="13"/>
-      <c r="E23" s="9"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="16"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="13"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="16"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -8058,76 +8058,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -11136,86 +11136,86 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
+      <c r="A2" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11240,7 +11240,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -11268,52 +11268,52 @@
       <c r="Z1" s="15"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11335,7 +11335,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>118</v>
@@ -11349,140 +11349,140 @@
       <c r="F1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>1.0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>47</v>
+      <c r="C3" s="5" t="s">
+        <v>26</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>1.0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>1.0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>113</v>
+      <c r="F4" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>1.0</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>48</v>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>1.0</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="10">
         <v>2.0</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11511,7 +11511,7 @@
         <v>132</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>133</v>
@@ -11542,76 +11542,76 @@
       <c r="Z1" s="18"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="4" t="b">
+      <c r="D2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="4" t="b">
+      <c r="D3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="6" t="b">
+      <c r="D4" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="10">
         <v>2.0</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11647,7 +11647,7 @@
         <v>143</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>144</v>
@@ -11676,11 +11676,11 @@
       <c r="AA1" s="22"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="str">
+      <c r="A2" s="5" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C2" s="23">
@@ -11714,11 +11714,11 @@
       <c r="AA2" s="25"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="str">
+      <c r="A3" s="5" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C3" s="23">
@@ -11752,11 +11752,11 @@
       <c r="AA3" s="25"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="str">
+      <c r="A4" s="5" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C4" s="23">
@@ -11790,11 +11790,11 @@
       <c r="AA4" s="25"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="str">
+      <c r="A5" s="5" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C5" s="23">
@@ -11828,11 +11828,11 @@
       <c r="AA5" s="25"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="str">
+      <c r="A6" s="5" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="23">
@@ -11866,11 +11866,11 @@
       <c r="AA6" s="25"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="str">
+      <c r="A7" s="5" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C7" s="23">
@@ -11953,7 +11953,7 @@
         <v>129</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="24" t="str">
@@ -12226,7 +12226,7 @@
         <v>129</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="24" t="str">
@@ -12499,7 +12499,7 @@
         <v>129</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="24" t="str">
@@ -12608,17 +12608,17 @@
       <c r="AA25" s="29"/>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="str">
+      <c r="A26" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="10" t="s">
         <v>122</v>
       </c>
       <c r="C26" s="33">
         <v>100.0</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="24" t="str">
         <f>vlookup(B26,TurtleCommands!A$2:C31,3,false)</f>
         <v>Distance</v>
@@ -12647,17 +12647,17 @@
       <c r="AA26" s="25"/>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="str">
+      <c r="A27" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C27" s="33">
         <v>90.0</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="24" t="str">
         <f>vlookup(B27,TurtleCommands!A$2:C32,3,false)</f>
         <v>Degrees</v>
@@ -12686,17 +12686,17 @@
       <c r="AA27" s="25"/>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="str">
+      <c r="A28" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="10" t="s">
         <v>122</v>
       </c>
       <c r="C28" s="33">
         <v>100.0</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="24" t="str">
         <f>vlookup(B28,TurtleCommands!A$2:C33,3,false)</f>
         <v>Distance</v>
@@ -12725,17 +12725,17 @@
       <c r="AA28" s="25"/>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="str">
+      <c r="A29" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C29" s="33">
         <v>90.0</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="24" t="str">
         <f>vlookup(B29,TurtleCommands!A$2:C34,3,false)</f>
         <v>Degrees</v>
@@ -12764,17 +12764,17 @@
       <c r="AA29" s="25"/>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="str">
+      <c r="A30" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="10" t="s">
         <v>122</v>
       </c>
       <c r="C30" s="33">
         <v>100.0</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="24" t="str">
         <f>vlookup(B30,TurtleCommands!A$2:C35,3,false)</f>
         <v>Distance</v>
@@ -12803,17 +12803,17 @@
       <c r="AA30" s="25"/>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="str">
+      <c r="A31" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C31" s="33">
         <v>90.0</v>
       </c>
-      <c r="D31" s="8"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="24" t="str">
         <f>vlookup(B31,TurtleCommands!A$2:C36,3,false)</f>
         <v>Degrees</v>
@@ -12842,17 +12842,17 @@
       <c r="AA31" s="25"/>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="str">
+      <c r="A32" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="10" t="s">
         <v>122</v>
       </c>
       <c r="C32" s="33">
         <v>100.0</v>
       </c>
-      <c r="D32" s="8"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="24" t="str">
         <f>vlookup(B32,TurtleCommands!A$2:C37,3,false)</f>
         <v>Distance</v>
@@ -12881,17 +12881,17 @@
       <c r="AA32" s="25"/>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="str">
+      <c r="A33" s="10" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C33" s="33">
         <v>90.0</v>
       </c>
-      <c r="D33" s="8"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="24" t="str">
         <f>vlookup(B33,TurtleCommands!A$2:C38,3,false)</f>
         <v>Degrees</v>

</xml_diff>

<commit_message>
Continued improving API ways of looking at a turtle.
</commit_message>
<xml_diff>
--- a/SSoT/twolaat.xlsx
+++ b/SSoT/twolaat.xlsx
@@ -22,13 +22,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>WayNumber</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>InitialValue</t>
+  </si>
+  <si>
+    <t>WayNumber</t>
   </si>
   <si>
     <t>DisplayWayNumber</t>
@@ -37,34 +37,16 @@
     <t>MainFileName</t>
   </si>
   <si>
+    <t>HexValue</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>HexValue</t>
+    <t>Black</t>
   </si>
   <si>
     <t>Position</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Advantages</t>
-  </si>
-  <si>
-    <t>Disadvantages</t>
-  </si>
-  <si>
-    <t>0x0</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
-    <t>Degrees</t>
-  </si>
-  <si>
-    <t>Black</t>
   </si>
   <si>
     <t>#000000</t>
@@ -82,10 +64,25 @@
     <t>#0000FF</t>
   </si>
   <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Advantages</t>
+  </si>
+  <si>
+    <t>Disadvantages</t>
+  </si>
+  <si>
     <t>W01</t>
   </si>
   <si>
-    <t>Green</t>
+    <t>#00FF00</t>
+  </si>
+  <si>
+    <t>0x0</t>
   </si>
   <si>
     <t>Way 01</t>
@@ -100,11 +97,17 @@
     <t>Simple OO -- a class with mutable state</t>
   </si>
   <si>
-    <t>#00FF00</t>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Degrees</t>
   </si>
   <si>
     <t>In this design, a simple OO class represents the turtle,
 and the client talks to the turtle directly.</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
   <si>
     <t>W02</t>
@@ -116,16 +119,13 @@
     <t>02-FPTurtle.fsx</t>
   </si>
   <si>
+    <t>PenState</t>
+  </si>
+  <si>
     <t>FPTurtle</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
     <t>Simple FP - a module of functions with immutable state</t>
-  </si>
-  <si>
-    <t>PenState</t>
   </si>
   <si>
     <t>In this design, the turtle state is immutable. A module contains functions that return a new turtle state,
@@ -154,6 +154,9 @@
 input and returns a Result containing any errors.</t>
   </si>
   <si>
+    <t>Down</t>
+  </si>
+  <si>
     <t>W04</t>
   </si>
   <si>
@@ -167,9 +170,6 @@
   </si>
   <si>
     <t>API (OO/FP hybrid approach) -- OO API calling stateless functions</t>
-  </si>
-  <si>
-    <t>Down</t>
   </si>
   <si>
     <t>In this design, an API layer communicates with pure turtle functions
@@ -215,7 +215,22 @@
 The client injects a specific turtle implementation via the API's constructor.</t>
   </si>
   <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>The pen is up (not drawing)</t>
+  </si>
+  <si>
+    <t>The pne is down (drawing)</t>
+  </si>
+  <si>
+    <t>Moving</t>
+  </si>
+  <si>
     <t>06-DependencyInjection_Interface-2.fsx</t>
+  </si>
+  <si>
+    <t>The pen is in motion</t>
   </si>
   <si>
     <t>DependencyInjection_Interface2</t>
@@ -391,24 +406,9 @@
     <t>API with capabilities</t>
   </si>
   <si>
-    <t>Up</t>
-  </si>
-  <si>
     <t>In this design, the turtle exposes a list of functions (capabilities) after each action.
 These are the ONLY actions available to the client
 More on capability-based security at http://fsharpforfunandprofit.com/posts/capability-based-security/</t>
-  </si>
-  <si>
-    <t>The pen is up (not drawing)</t>
-  </si>
-  <si>
-    <t>The pne is down (drawing)</t>
-  </si>
-  <si>
-    <t>Moving</t>
-  </si>
-  <si>
-    <t>The pen is in motion</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -465,22 +465,19 @@
     <t>int</t>
   </si>
   <si>
+    <t>DisplayName</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
     <t>PredefinedScript</t>
   </si>
   <si>
     <t>Command</t>
   </si>
   <si>
-    <t>DisplayName</t>
-  </si>
-  <si>
     <t>Argument</t>
-  </si>
-  <si>
-    <t>IsActive</t>
-  </si>
-  <si>
-    <t>ArgumentType</t>
   </si>
   <si>
     <t>Triangle</t>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>Draw three paralell lines of length 100, 50 pixels apart</t>
+  </si>
+  <si>
+    <t>ArgumentType</t>
   </si>
   <si>
     <t>Box</t>
@@ -561,14 +561,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -601,29 +601,29 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -639,34 +639,34 @@
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -674,7 +674,7 @@
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -731,7 +731,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -742,17 +742,17 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -777,446 +777,446 @@
       <c r="AC1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>21</v>
+      <c r="A2" s="8" t="s">
+        <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>49</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="5" t="str">
+      <c r="B6" s="4" t="str">
         <f t="shared" ref="B6:B19" si="1">CONCATENATE("Way ",right(A6,2))</f>
         <v>Way 05</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="5" t="str">
+      <c r="B7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 06</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="5" t="str">
+      <c r="B8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 06</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>60</v>
+      <c r="C8" s="4" t="s">
+        <v>64</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>61</v>
+      <c r="D8" s="4" t="s">
+        <v>66</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>62</v>
+      <c r="E8" s="10" t="s">
+        <v>67</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>63</v>
+      <c r="A9" s="8" t="s">
+        <v>68</v>
       </c>
-      <c r="B9" s="5" t="str">
+      <c r="B9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 07</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>64</v>
+      <c r="C9" s="4" t="s">
+        <v>69</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>65</v>
+      <c r="D9" s="4" t="s">
+        <v>70</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>66</v>
+      <c r="E9" s="10" t="s">
+        <v>71</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>67</v>
+      <c r="F9" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
-        <v>63</v>
+      <c r="A10" s="8" t="s">
+        <v>68</v>
       </c>
-      <c r="B10" s="5" t="str">
+      <c r="B10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 07</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>68</v>
+      <c r="C10" s="4" t="s">
+        <v>73</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>69</v>
+      <c r="D10" s="4" t="s">
+        <v>74</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>70</v>
+      <c r="E10" s="10" t="s">
+        <v>75</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>67</v>
+      <c r="F10" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>71</v>
+      <c r="A11" s="8" t="s">
+        <v>76</v>
       </c>
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 08</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>72</v>
+      <c r="C11" s="4" t="s">
+        <v>77</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>73</v>
+      <c r="D11" s="4" t="s">
+        <v>78</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>74</v>
+      <c r="E11" s="10" t="s">
+        <v>79</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>75</v>
+      <c r="F11" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="13"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>76</v>
+      <c r="A12" s="8" t="s">
+        <v>81</v>
       </c>
-      <c r="B12" s="5" t="str">
+      <c r="B12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 09</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>77</v>
+      <c r="C12" s="4" t="s">
+        <v>82</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>78</v>
+      <c r="D12" s="4" t="s">
+        <v>83</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>79</v>
+      <c r="E12" s="10" t="s">
+        <v>84</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>80</v>
+      <c r="F12" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>81</v>
+      <c r="A13" s="8" t="s">
+        <v>86</v>
       </c>
-      <c r="B13" s="5" t="str">
+      <c r="B13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 10</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>82</v>
+      <c r="C13" s="4" t="s">
+        <v>87</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>83</v>
+      <c r="D13" s="4" t="s">
+        <v>88</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>84</v>
+      <c r="E13" s="10" t="s">
+        <v>89</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>85</v>
+      <c r="F13" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>86</v>
+      <c r="A14" s="8" t="s">
+        <v>91</v>
       </c>
-      <c r="B14" s="5" t="str">
+      <c r="B14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 11</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>87</v>
+      <c r="C14" s="4" t="s">
+        <v>92</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>88</v>
+      <c r="D14" s="4" t="s">
+        <v>93</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>89</v>
+      <c r="E14" s="10" t="s">
+        <v>94</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>90</v>
+      <c r="F14" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
-        <v>91</v>
+      <c r="A15" s="8" t="s">
+        <v>96</v>
       </c>
-      <c r="B15" s="5" t="str">
+      <c r="B15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 12</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>92</v>
+      <c r="C15" s="4" t="s">
+        <v>97</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>93</v>
+      <c r="D15" s="4" t="s">
+        <v>98</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>94</v>
+      <c r="E15" s="10" t="s">
+        <v>99</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>95</v>
+      <c r="F15" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
-        <v>96</v>
+      <c r="A16" s="8" t="s">
+        <v>101</v>
       </c>
-      <c r="B16" s="5" t="str">
+      <c r="B16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 13</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>97</v>
+      <c r="C16" s="4" t="s">
+        <v>102</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>98</v>
+      <c r="D16" s="4" t="s">
+        <v>103</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>99</v>
+      <c r="E16" s="10" t="s">
+        <v>104</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>100</v>
+      <c r="F16" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
-        <v>96</v>
+      <c r="A17" s="8" t="s">
+        <v>101</v>
       </c>
-      <c r="B17" s="5" t="str">
+      <c r="B17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 13</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>101</v>
+      <c r="C17" s="4" t="s">
+        <v>106</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>102</v>
+      <c r="D17" s="4" t="s">
+        <v>107</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>99</v>
+      <c r="E17" s="10" t="s">
+        <v>104</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>100</v>
+      <c r="F17" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
-        <v>103</v>
+      <c r="A18" s="8" t="s">
+        <v>108</v>
       </c>
-      <c r="B18" s="5" t="str">
+      <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 14</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>104</v>
+      <c r="C18" s="4" t="s">
+        <v>109</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>105</v>
+      <c r="D18" s="4" t="s">
+        <v>110</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>106</v>
+      <c r="E18" s="10" t="s">
+        <v>111</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>107</v>
+      <c r="F18" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
-        <v>108</v>
+      <c r="A19" s="8" t="s">
+        <v>113</v>
       </c>
-      <c r="B19" s="5" t="str">
+      <c r="B19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Way 15</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>109</v>
+      <c r="C19" s="4" t="s">
+        <v>114</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>110</v>
+      <c r="D19" s="4" t="s">
+        <v>115</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>111</v>
+      <c r="E19" s="10" t="s">
+        <v>116</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>113</v>
+      <c r="F19" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
     <row r="20">
       <c r="A20" s="13"/>
-      <c r="E20" s="9"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="16"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21">
       <c r="A21" s="13"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="16"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
     <row r="22">
       <c r="A22" s="13"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="16"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
     <row r="23">
       <c r="A23" s="13"/>
-      <c r="E23" s="9"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="16"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="13"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="16"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -8070,10 +8070,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -8100,47 +8100,47 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
+      <c r="A2" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
+      <c r="C2" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
+      <c r="A3" s="4" t="s">
+        <v>26</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C3" s="11">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>48</v>
+      <c r="C5" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -11148,7 +11148,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -11175,59 +11175,59 @@
       <c r="Y1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11252,7 +11252,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -11280,52 +11280,52 @@
       <c r="Z1" s="15"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>112</v>
+      <c r="A2" s="4" t="s">
+        <v>60</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>114</v>
+      <c r="B2" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>48</v>
+      <c r="A3" s="4" t="s">
+        <v>43</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>115</v>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>116</v>
+      <c r="A4" s="6" t="s">
+        <v>63</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>117</v>
+      <c r="B4" s="6" t="s">
+        <v>65</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11347,7 +11347,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>118</v>
@@ -11385,131 +11385,131 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1.0</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1.0</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>1.0</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>112</v>
+      <c r="G4" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1.0</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>48</v>
+      <c r="G5" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>33</v>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1.0</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>2.0</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11535,110 +11535,110 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>142</v>
+      <c r="D2" s="4" t="b">
+        <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="5" t="b">
+      <c r="B3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E3" s="4">
         <v>1.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="8" t="b">
+      <c r="D4" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>2.0</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11665,19 +11665,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="17" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" s="18" t="s">
         <v>139</v>
       </c>
+      <c r="C1" s="19" t="s">
+        <v>140</v>
+      </c>
       <c r="D1" s="17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -11703,11 +11703,11 @@
       <c r="AA1" s="22"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="4" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C2" s="23">
@@ -11741,11 +11741,11 @@
       <c r="AA2" s="25"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C3" s="23">
@@ -11779,11 +11779,11 @@
       <c r="AA3" s="25"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C4" s="23">
@@ -11817,11 +11817,11 @@
       <c r="AA4" s="25"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="4" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C5" s="23">
@@ -11855,11 +11855,11 @@
       <c r="AA5" s="25"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="4" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C6" s="23">
@@ -11893,11 +11893,11 @@
       <c r="AA6" s="25"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="4" t="str">
         <f>PredifinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C7" s="23">
@@ -11980,7 +11980,7 @@
         <v>131</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="24" t="str">
@@ -12253,7 +12253,7 @@
         <v>131</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="24" t="str">
@@ -12526,7 +12526,7 @@
         <v>131</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="24" t="str">
@@ -12635,17 +12635,17 @@
       <c r="AA25" s="29"/>
     </row>
     <row r="26">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C26" s="33">
         <v>100.0</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="24" t="str">
         <f>vlookup(B26,TurtleCommands!A$2:C31,3,false)</f>
         <v>Distance</v>
@@ -12674,17 +12674,17 @@
       <c r="AA26" s="25"/>
     </row>
     <row r="27">
-      <c r="A27" s="8" t="str">
+      <c r="A27" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C27" s="33">
         <v>90.0</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="24" t="str">
         <f>vlookup(B27,TurtleCommands!A$2:C32,3,false)</f>
         <v>Degrees</v>
@@ -12713,17 +12713,17 @@
       <c r="AA27" s="25"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C28" s="33">
         <v>100.0</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="7"/>
       <c r="E28" s="24" t="str">
         <f>vlookup(B28,TurtleCommands!A$2:C33,3,false)</f>
         <v>Distance</v>
@@ -12752,17 +12752,17 @@
       <c r="AA28" s="25"/>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="str">
+      <c r="A29" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C29" s="33">
         <v>90.0</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="7"/>
       <c r="E29" s="24" t="str">
         <f>vlookup(B29,TurtleCommands!A$2:C34,3,false)</f>
         <v>Degrees</v>
@@ -12791,17 +12791,17 @@
       <c r="AA29" s="25"/>
     </row>
     <row r="30">
-      <c r="A30" s="8" t="str">
+      <c r="A30" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C30" s="33">
         <v>100.0</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="7"/>
       <c r="E30" s="24" t="str">
         <f>vlookup(B30,TurtleCommands!A$2:C35,3,false)</f>
         <v>Distance</v>
@@ -12830,17 +12830,17 @@
       <c r="AA30" s="25"/>
     </row>
     <row r="31">
-      <c r="A31" s="8" t="str">
+      <c r="A31" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C31" s="33">
         <v>90.0</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="24" t="str">
         <f>vlookup(B31,TurtleCommands!A$2:C36,3,false)</f>
         <v>Degrees</v>
@@ -12869,17 +12869,17 @@
       <c r="AA31" s="25"/>
     </row>
     <row r="32">
-      <c r="A32" s="8" t="str">
+      <c r="A32" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C32" s="33">
         <v>100.0</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="7"/>
       <c r="E32" s="24" t="str">
         <f>vlookup(B32,TurtleCommands!A$2:C37,3,false)</f>
         <v>Distance</v>
@@ -12908,17 +12908,17 @@
       <c r="AA32" s="25"/>
     </row>
     <row r="33">
-      <c r="A33" s="8" t="str">
+      <c r="A33" s="6" t="str">
         <f>PredifinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C33" s="33">
         <v>90.0</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="7"/>
       <c r="E33" s="24" t="str">
         <f>vlookup(B33,TurtleCommands!A$2:C38,3,false)</f>
         <v>Degrees</v>

</xml_diff>

<commit_message>
Updated git ignore settings - and project docs getting re-created.
</commit_message>
<xml_diff>
--- a/SSoT/twolaat.xlsx
+++ b/SSoT/twolaat.xlsx
@@ -22,22 +22,25 @@
     <t>WayNumber</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>DisplayWayNumber</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>HexValue</t>
   </si>
   <si>
     <t>MainFileName</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
     <t>InitialValue</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>Notes</t>
@@ -49,19 +52,13 @@
     <t>Disadvantages</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>HexValue</t>
-  </si>
-  <si>
     <t>W01</t>
   </si>
   <si>
     <t>Black</t>
   </si>
   <si>
-    <t>0x0</t>
+    <t>Position</t>
   </si>
   <si>
     <t>Way 01</t>
@@ -70,10 +67,31 @@
     <t>01-OOTurtle.fsx</t>
   </si>
   <si>
+    <t>#000000</t>
+  </si>
+  <si>
     <t>OOTurtle</t>
   </si>
   <si>
+    <t>0x0</t>
+  </si>
+  <si>
     <t>Simple OO -- a class with mutable state</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>#FF0000</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>#0000FF</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
   <si>
     <t>Angle</t>
@@ -82,17 +100,23 @@
     <t>Degrees</t>
   </si>
   <si>
-    <t>In this design, a simple OO class represents the turtle,
-and the client talks to the turtle directly.</t>
+    <t>#00FF00</t>
   </si>
   <si>
     <t>Color</t>
   </si>
   <si>
-    <t>W02</t>
+    <t>PenState</t>
   </si>
   <si>
-    <t>PenState</t>
+    <t>In this design, a simple OO class represents the turtle,
+and the client talks to the turtle directly.</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>W02</t>
   </si>
   <si>
     <t>Way 02</t>
@@ -104,16 +128,7 @@
     <t>FPTurtle</t>
   </si>
   <si>
-    <t>#000000</t>
-  </si>
-  <si>
     <t>Simple FP - a module of functions with immutable state</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>#FF0000</t>
   </si>
   <si>
     <t>In this design, the turtle state is immutable. A module contains functions that return a new turtle state,
@@ -121,16 +136,7 @@
 The client must keep track of the current state and pass it into the next function call.</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>W03</t>
-  </si>
-  <si>
-    <t>#0000FF</t>
-  </si>
-  <si>
-    <t>Green</t>
   </si>
   <si>
     <t>Way 03</t>
@@ -149,9 +155,6 @@
 and the client talks to the API layer.
 The input to the API are strings, and so the API validates the
 input and returns a Result containing any errors.</t>
-  </si>
-  <si>
-    <t>Down</t>
   </si>
   <si>
     <t>W04</t>
@@ -176,9 +179,6 @@
   </si>
   <si>
     <t>W05</t>
-  </si>
-  <si>
-    <t>#00FF00</t>
   </si>
   <si>
     <t>05-TurtleAgent.fsx</t>
@@ -604,28 +604,28 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,25 +734,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -777,410 +777,410 @@
       <c r="AC1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>12</v>
+      <c r="A2" s="5" t="s">
+        <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>18</v>
+      <c r="E2" s="11" t="s">
+        <v>19</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>21</v>
+      <c r="F2" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>23</v>
+      <c r="A3" s="5" t="s">
+        <v>32</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>26</v>
+      <c r="C3" s="6" t="s">
+        <v>34</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>27</v>
+      <c r="D3" s="6" t="s">
+        <v>35</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>29</v>
+      <c r="E3" s="11" t="s">
+        <v>36</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>32</v>
+      <c r="F3" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>41</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="11" t="s">
         <v>48</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>49</v>
+      <c r="A6" s="5" t="s">
+        <v>50</v>
       </c>
-      <c r="B6" s="5" t="str">
+      <c r="B6" s="6" t="str">
         <f t="shared" ref="B6:B19" si="1">CONCATENATE("Way ",right(A6,2))</f>
         <v>Way 05</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="5" t="str">
+      <c r="B7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 06</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="5" t="str">
+      <c r="B8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 06</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="5" t="str">
+      <c r="B9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 07</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="11" t="s">
         <v>67</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="5" t="str">
+      <c r="B10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 07</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="11" t="s">
         <v>67</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 08</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="11" t="s">
         <v>75</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="13"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="5" t="str">
+      <c r="B12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 09</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="11" t="s">
         <v>80</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="5" t="str">
+      <c r="B13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 10</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="11" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="5" t="str">
+      <c r="B14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="11" t="s">
         <v>90</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="5" t="str">
+      <c r="B15" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 12</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="11" t="s">
         <v>95</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="5" t="str">
+      <c r="B16" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 13</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="11" t="s">
         <v>100</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="5" t="str">
+      <c r="B17" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 13</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="11" t="s">
         <v>100</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="5" t="str">
+      <c r="B18" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 14</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="11" t="s">
         <v>107</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="5" t="str">
+      <c r="B19" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 15</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="11" t="s">
         <v>112</v>
       </c>
       <c r="G19" s="13"/>
@@ -1188,35 +1188,35 @@
     </row>
     <row r="20">
       <c r="A20" s="13"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="14"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21">
       <c r="A21" s="13"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="14"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
     <row r="22">
       <c r="A22" s="13"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="14"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
     <row r="23">
       <c r="A23" s="13"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="14"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="13"/>
-      <c r="E24" s="8"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="14"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -8067,7 +8067,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -8100,47 +8100,47 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>10</v>
+      <c r="A2" s="6" t="s">
+        <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>19</v>
+      <c r="A3" s="6" t="s">
+        <v>25</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
+      <c r="B3" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C3" s="9">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
+      <c r="A4" s="6" t="s">
+        <v>28</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>22</v>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>24</v>
+      <c r="A5" s="6" t="s">
+        <v>29</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>24</v>
+      <c r="B5" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
@@ -11145,10 +11145,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -11175,59 +11175,59 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
+      <c r="A2" s="6" t="s">
+        <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>28</v>
+      <c r="B2" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>20</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>31</v>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>33</v>
+      <c r="A4" s="6" t="s">
+        <v>22</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>35</v>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>36</v>
+      <c r="A5" s="8" t="s">
+        <v>24</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>50</v>
+      <c r="B5" s="8" t="s">
+        <v>27</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11249,10 +11249,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -11280,52 +11280,52 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>42</v>
+      <c r="A3" s="6" t="s">
+        <v>31</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11344,10 +11344,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>118</v>
@@ -11385,131 +11385,131 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>1.0</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
+      <c r="C3" s="6" t="s">
+        <v>26</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>1.0</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>1.0</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>1.0</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>42</v>
+      <c r="G5" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>22</v>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>1.0</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>2.0</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
     </row>
     <row r="8">
-      <c r="A8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11532,13 +11532,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>136</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>137</v>
@@ -11569,76 +11569,76 @@
       <c r="Z1" s="18"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="5" t="b">
+      <c r="D2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="5" t="b">
+      <c r="D3" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="11" t="b">
+      <c r="D4" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>2.0</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11674,7 +11674,7 @@
         <v>147</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>148</v>
@@ -11703,11 +11703,11 @@
       <c r="AA1" s="22"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="6" t="str">
         <f>PredefinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C2" s="23">
@@ -11741,11 +11741,11 @@
       <c r="AA2" s="25"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="6" t="str">
         <f>PredefinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C3" s="23">
@@ -11779,11 +11779,11 @@
       <c r="AA3" s="25"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="6" t="str">
         <f>PredefinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C4" s="23">
@@ -11817,11 +11817,11 @@
       <c r="AA4" s="25"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="6" t="str">
         <f>PredefinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C5" s="23">
@@ -11855,11 +11855,11 @@
       <c r="AA5" s="25"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="6" t="str">
         <f>PredefinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C6" s="23">
@@ -11893,11 +11893,11 @@
       <c r="AA6" s="25"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="6" t="str">
         <f>PredefinedScripts!A$2</f>
         <v>Triangle</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C7" s="23">
@@ -11980,7 +11980,7 @@
         <v>131</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="24" t="str">
@@ -12253,7 +12253,7 @@
         <v>131</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="24" t="str">
@@ -12526,7 +12526,7 @@
         <v>131</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="24" t="str">
@@ -12635,17 +12635,17 @@
       <c r="AA25" s="29"/>
     </row>
     <row r="26">
-      <c r="A26" s="11" t="str">
+      <c r="A26" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C26" s="33">
         <v>100.0</v>
       </c>
-      <c r="D26" s="12"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="24" t="str">
         <f>vlookup(B26,TurtleCommands!A$2:C31,3,false)</f>
         <v>Distance</v>
@@ -12674,17 +12674,17 @@
       <c r="AA26" s="25"/>
     </row>
     <row r="27">
-      <c r="A27" s="11" t="str">
+      <c r="A27" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C27" s="33">
         <v>90.0</v>
       </c>
-      <c r="D27" s="12"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="24" t="str">
         <f>vlookup(B27,TurtleCommands!A$2:C32,3,false)</f>
         <v>Degrees</v>
@@ -12713,17 +12713,17 @@
       <c r="AA27" s="25"/>
     </row>
     <row r="28">
-      <c r="A28" s="11" t="str">
+      <c r="A28" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C28" s="33">
         <v>100.0</v>
       </c>
-      <c r="D28" s="12"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="24" t="str">
         <f>vlookup(B28,TurtleCommands!A$2:C33,3,false)</f>
         <v>Distance</v>
@@ -12752,17 +12752,17 @@
       <c r="AA28" s="25"/>
     </row>
     <row r="29">
-      <c r="A29" s="11" t="str">
+      <c r="A29" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C29" s="33">
         <v>90.0</v>
       </c>
-      <c r="D29" s="12"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="24" t="str">
         <f>vlookup(B29,TurtleCommands!A$2:C34,3,false)</f>
         <v>Degrees</v>
@@ -12791,17 +12791,17 @@
       <c r="AA29" s="25"/>
     </row>
     <row r="30">
-      <c r="A30" s="11" t="str">
+      <c r="A30" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C30" s="33">
         <v>100.0</v>
       </c>
-      <c r="D30" s="12"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="24" t="str">
         <f>vlookup(B30,TurtleCommands!A$2:C35,3,false)</f>
         <v>Distance</v>
@@ -12830,17 +12830,17 @@
       <c r="AA30" s="25"/>
     </row>
     <row r="31">
-      <c r="A31" s="11" t="str">
+      <c r="A31" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C31" s="33">
         <v>90.0</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="24" t="str">
         <f>vlookup(B31,TurtleCommands!A$2:C36,3,false)</f>
         <v>Degrees</v>
@@ -12869,17 +12869,17 @@
       <c r="AA31" s="25"/>
     </row>
     <row r="32">
-      <c r="A32" s="11" t="str">
+      <c r="A32" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C32" s="33">
         <v>100.0</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="24" t="str">
         <f>vlookup(B32,TurtleCommands!A$2:C37,3,false)</f>
         <v>Distance</v>
@@ -12908,17 +12908,17 @@
       <c r="AA32" s="25"/>
     </row>
     <row r="33">
-      <c r="A33" s="11" t="str">
+      <c r="A33" s="8" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C33" s="33">
         <v>90.0</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="24" t="str">
         <f>vlookup(B33,TurtleCommands!A$2:C38,3,false)</f>
         <v>Degrees</v>

</xml_diff>

<commit_message>
Replacing original readme with "One Way of Looking At 13..."
</commit_message>
<xml_diff>
--- a/SSoT/twolaat.xlsx
+++ b/SSoT/twolaat.xlsx
@@ -25,22 +25,13 @@
     <t>DisplayWayNumber</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>MainFileName</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>InitialValue</t>
-  </si>
-  <si>
-    <t>HexValue</t>
   </si>
   <si>
     <t>Notes</t>
@@ -55,13 +46,28 @@
     <t>W01</t>
   </si>
   <si>
-    <t>Black</t>
+    <t>Way 01</t>
   </si>
   <si>
-    <t>Position</t>
+    <t>01-OOTurtle.fsx</t>
   </si>
   <si>
-    <t>Way 01</t>
+    <t>OOTurtle</t>
+  </si>
+  <si>
+    <t>HexValue</t>
+  </si>
+  <si>
+    <t>Simple OO -- a class with mutable state</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>InitialValue</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
   <si>
     <t>#000000</t>
@@ -70,44 +76,29 @@
     <t>Red</t>
   </si>
   <si>
-    <t>01-OOTurtle.fsx</t>
-  </si>
-  <si>
     <t>#FF0000</t>
   </si>
   <si>
-    <t>OOTurtle</t>
-  </si>
-  <si>
     <t>Blue</t>
-  </si>
-  <si>
-    <t>Simple OO -- a class with mutable state</t>
-  </si>
-  <si>
-    <t>#0000FF</t>
-  </si>
-  <si>
-    <t>0x0</t>
-  </si>
-  <si>
-    <t>Green</t>
   </si>
   <si>
     <t>In this design, a simple OO class represents the turtle,
 and the client talks to the turtle directly.</t>
   </si>
   <si>
-    <t>Angle</t>
+    <t>#0000FF</t>
   </si>
   <si>
-    <t>Degrees</t>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>0x0</t>
   </si>
   <si>
     <t>W02</t>
-  </si>
-  <si>
-    <t>Color</t>
   </si>
   <si>
     <t>Way 02</t>
@@ -117,9 +108,6 @@
   </si>
   <si>
     <t>FPTurtle</t>
-  </si>
-  <si>
-    <t>PenState</t>
   </si>
   <si>
     <t>Simple FP - a module of functions with immutable state</t>
@@ -151,6 +139,9 @@
 input and returns a Result containing any errors.</t>
   </si>
   <si>
+    <t>#00FF00</t>
+  </si>
+  <si>
     <t>W04</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>API (OO/FP hybrid approach) -- OO API calling stateless functions</t>
   </si>
   <si>
-    <t>#00FF00</t>
-  </si>
-  <si>
     <t>In this design, an API layer communicates with pure turtle functions
 and the client talks to the API layer.
 The API layer manages the state (rather than the client) by storing a mutable turtle state.
@@ -176,6 +164,18 @@
   </si>
   <si>
     <t>W05</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>PenState</t>
   </si>
   <si>
     <t>Down</t>
@@ -297,9 +297,6 @@
     <t>Event sourcing -- Building state from a list of past events</t>
   </si>
   <si>
-    <t>Up</t>
-  </si>
-  <si>
     <t>In this design, the client sends a `Command` to a `CommandHandler`.
 The CommandHandler converts that to a list of events and stores them in an `EventStore`.
 In order to know how to process a Command, the CommandHandler builds the current state
@@ -307,19 +304,7 @@
 Neither the client nor the command handler needs to track state.  Only the EventStore is mutable.</t>
   </si>
   <si>
-    <t>The pen is up (not drawing)</t>
-  </si>
-  <si>
     <t>W11</t>
-  </si>
-  <si>
-    <t>The pne is down (drawing)</t>
-  </si>
-  <si>
-    <t>Moving</t>
-  </si>
-  <si>
-    <t>The pen is in motion</t>
   </si>
   <si>
     <t>11-FRP.fsx</t>
@@ -357,6 +342,12 @@
     <t>W13</t>
   </si>
   <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>The pen is up (not drawing)</t>
+  </si>
+  <si>
     <t>13-Interpreter-v1.fsx</t>
   </si>
   <si>
@@ -366,8 +357,17 @@
     <t>The interpreter pattern</t>
   </si>
   <si>
+    <t>The pne is down (drawing)</t>
+  </si>
+  <si>
+    <t>Moving</t>
+  </si>
+  <si>
     <t>In this design, the client builds a data structure (`TurtleProgram`) that represents the instructions.
 This Turtle Program can then interpreted later in various ways</t>
+  </si>
+  <si>
+    <t>The pen is in motion</t>
   </si>
   <si>
     <t>13-Interpreter-v2.fsx</t>
@@ -618,14 +618,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -670,17 +670,17 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -703,27 +703,27 @@
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -731,7 +731,7 @@
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -794,22 +794,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -835,95 +835,95 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6" t="str">
         <f t="shared" ref="B6:B19" si="1">CONCATENATE("Way ",right(A6,2))</f>
@@ -941,8 +941,8 @@
       <c r="F6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
@@ -964,8 +964,8 @@
       <c r="F7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
@@ -987,8 +987,8 @@
       <c r="F8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
@@ -1010,8 +1010,8 @@
       <c r="F9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
@@ -1033,8 +1033,8 @@
       <c r="F10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
@@ -1056,7 +1056,7 @@
       <c r="F11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="13"/>
     </row>
     <row r="12">
@@ -1100,83 +1100,83 @@
         <v>84</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 11</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B15" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 12</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B16" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Way 13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E16" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B17" s="6" t="str">
         <f t="shared" si="1"/>
@@ -1189,10 +1189,10 @@
         <v>107</v>
       </c>
       <c r="E17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -8124,13 +8124,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -8158,45 +8158,45 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="9">
+        <v>47</v>
+      </c>
+      <c r="C3" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -11202,10 +11202,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -11233,18 +11233,18 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -11256,35 +11256,35 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
+      <c r="B5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11306,10 +11306,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -11338,10 +11338,10 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
@@ -11349,40 +11349,40 @@
         <v>50</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
+      <c r="A4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -11406,10 +11406,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>118</v>
@@ -11494,7 +11494,7 @@
         <v>132</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>130</v>
@@ -11530,7 +11530,7 @@
         <v>135</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5">
@@ -11560,7 +11560,7 @@
         <v>139</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>140</v>
@@ -11578,53 +11578,53 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9">
         <v>2.0</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>0.0</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>360.0</v>
       </c>
-      <c r="J7" s="10" t="str">
+      <c r="J7" s="9" t="str">
         <f t="shared" si="1"/>
         <v>DrawPolygon</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
@@ -12269,13 +12269,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>156</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>157</v>
@@ -12340,42 +12340,42 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="10" t="b">
+      <c r="D4" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>2.0</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -12411,7 +12411,7 @@
         <v>166</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>167</v>
@@ -12717,7 +12717,7 @@
         <v>138</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="24" t="str">
@@ -12990,7 +12990,7 @@
         <v>138</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="24" t="str">
@@ -13372,17 +13372,17 @@
       <c r="AA25" s="29"/>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="str">
+      <c r="A26" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>127</v>
       </c>
       <c r="C26" s="33">
         <v>100.0</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="24" t="str">
         <f>vlookup(B26,TurtleCommands!A$2:C31,3,false)</f>
         <v>Distance</v>
@@ -13411,17 +13411,17 @@
       <c r="AA26" s="25"/>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="str">
+      <c r="A27" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C27" s="33">
         <v>90.0</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="24" t="str">
         <f>vlookup(B27,TurtleCommands!A$2:C32,3,false)</f>
         <v>Degrees</v>
@@ -13450,17 +13450,17 @@
       <c r="AA27" s="25"/>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="str">
+      <c r="A28" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>127</v>
       </c>
       <c r="C28" s="33">
         <v>100.0</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="24" t="str">
         <f>vlookup(B28,TurtleCommands!A$2:C33,3,false)</f>
         <v>Distance</v>
@@ -13489,17 +13489,17 @@
       <c r="AA28" s="25"/>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="str">
+      <c r="A29" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C29" s="33">
         <v>90.0</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="24" t="str">
         <f>vlookup(B29,TurtleCommands!A$2:C34,3,false)</f>
         <v>Degrees</v>
@@ -13528,17 +13528,17 @@
       <c r="AA29" s="25"/>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="str">
+      <c r="A30" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>127</v>
       </c>
       <c r="C30" s="33">
         <v>100.0</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="24" t="str">
         <f>vlookup(B30,TurtleCommands!A$2:C35,3,false)</f>
         <v>Distance</v>
@@ -13567,17 +13567,17 @@
       <c r="AA30" s="25"/>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="str">
+      <c r="A31" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C31" s="33">
         <v>90.0</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="24" t="str">
         <f>vlookup(B31,TurtleCommands!A$2:C36,3,false)</f>
         <v>Degrees</v>
@@ -13606,17 +13606,17 @@
       <c r="AA31" s="25"/>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="str">
+      <c r="A32" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>127</v>
       </c>
       <c r="C32" s="33">
         <v>100.0</v>
       </c>
-      <c r="D32" s="11"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="24" t="str">
         <f>vlookup(B32,TurtleCommands!A$2:C37,3,false)</f>
         <v>Distance</v>
@@ -13645,17 +13645,17 @@
       <c r="AA32" s="25"/>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="str">
+      <c r="A33" s="9" t="str">
         <f>PredefinedScripts!A$4</f>
         <v>Box</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C33" s="33">
         <v>90.0</v>
       </c>
-      <c r="D33" s="11"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="24" t="str">
         <f>vlookup(B33,TurtleCommands!A$2:C38,3,false)</f>
         <v>Degrees</v>

</xml_diff>